<commit_message>
add datepicker to "AvailableHour" exported file
add datepicker to "AvailableHour" exported file form.
update "AvailableHour" listing view.
</commit_message>
<xml_diff>
--- a/GRis/Content/ExcelTemplates/ServerAvailableHoursTemplate.xlsx
+++ b/GRis/Content/ExcelTemplates/ServerAvailableHoursTemplate.xlsx
@@ -19,15 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Server ID</t>
   </si>
   <si>
     <t>Server Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Date</t>
@@ -40,14 +37,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -79,16 +71,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -404,40 +394,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.77734375" customWidth="1"/>
     <col min="3" max="3" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="21" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
generate "Staff Percentages" report.
</commit_message>
<xml_diff>
--- a/GRis/Content/ExcelTemplates/ServerAvailableHoursTemplate.xlsx
+++ b/GRis/Content/ExcelTemplates/ServerAvailableHoursTemplate.xlsx
@@ -37,7 +37,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -50,6 +50,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -59,7 +67,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -67,21 +75,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -394,35 +413,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21" style="2" customWidth="1"/>
     <col min="5" max="21" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>